<commit_message>
- Added: 0114-Asset-CSWNEQPFUNCTN to populate maxdomain STE_CSWNEQPFUNCTN values.
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/STR(DM-Master)-Appendix B - Test and PR Summary_Master_Data_09012025.xlsx
+++ b/Integration Services Project2/notes/STR(DM-Master)-Appendix B - Test and PR Summary_Master_Data_09012025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337034E3-C54A-45B4-90E9-8A3BCD7B6753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5A8FC4-47C0-4AF1-9FC3-3BDB1DD74070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6080,8 +6080,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:W2230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="W79" sqref="W79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>